<commit_message>
Modified and added several folders and files
</commit_message>
<xml_diff>
--- a/Project2-SystemOverview.xlsx
+++ b/Project2-SystemOverview.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\EvolveU\Project2\POS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1C7E6F2-4469-4559-9EEE-336E4AA1F4AF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1434F452-6FE0-4046-9610-5DEF08AA7170}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -1246,25 +1246,25 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-CA" sz="1100"/>
-            <a:t>- ID</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-CA" sz="1100"/>
-            <a:t>- Name</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-CA" sz="1100"/>
-            <a:t>- Address1</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-CA" sz="1100"/>
-            <a:t>- Address2</a:t>
+            <a:t>- id</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1100"/>
+            <a:t>- name</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1100"/>
+            <a:t>- address1</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1100"/>
+            <a:t>- address2</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -1274,49 +1274,49 @@
           </a:r>
           <a:r>
             <a:rPr lang="en-CA" sz="1100" baseline="0"/>
-            <a:t> City</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-CA" sz="1100" baseline="0"/>
-            <a:t>- Province</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-CA" sz="1100"/>
-            <a:t>- PostalCode</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-CA" sz="1100"/>
-            <a:t>- PhoneNumber</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-CA" sz="1100"/>
-            <a:t>- ContactPerson</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-CA" sz="1100"/>
-            <a:t>- Active</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-CA" sz="1100"/>
-            <a:t>- DateAdded</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-CA" sz="1100"/>
-            <a:t>- LastUpdateDate</a:t>
+            <a:t> city</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1100" baseline="0"/>
+            <a:t>- province</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1100"/>
+            <a:t>- postalCode</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1100"/>
+            <a:t>- phoneNumber</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1100"/>
+            <a:t>- contactPerson</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1100"/>
+            <a:t>- active</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1100"/>
+            <a:t>- dateAdded</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1100"/>
+            <a:t>- lastUpdateDate</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -1392,49 +1392,55 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-CA" sz="1100"/>
-            <a:t>- ID</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-CA" sz="1100"/>
-            <a:t>- Name</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-CA" sz="1100"/>
-            <a:t>- Description</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-CA" sz="1100"/>
-            <a:t>- ProductCategoryID</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-CA" sz="1100"/>
-            <a:t>- SupplierID</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-CA" sz="1100"/>
-            <a:t>- Active</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-CA" sz="1100"/>
-            <a:t>- DateAdded</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-CA" sz="1100"/>
-            <a:t>- Last</a:t>
+            <a:t>- id</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1100"/>
+            <a:t>- name</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1100"/>
+            <a:t>- description</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1100"/>
+            <a:t>- productCategoryId</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1100"/>
+            <a:t>- unitPrice</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1100"/>
+            <a:t>- supplierId</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1100"/>
+            <a:t>- active</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1100"/>
+            <a:t>- dateAdded</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1100"/>
+            <a:t>- last</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-CA" sz="1100" baseline="0"/>
@@ -1515,25 +1521,25 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-CA" sz="1100"/>
-            <a:t>- ID</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-CA" sz="1100"/>
-            <a:t>- CompanyName</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-CA" sz="1100"/>
-            <a:t>- Address1</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-CA" sz="1100"/>
-            <a:t>- Address</a:t>
+            <a:t>- id</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1100"/>
+            <a:t>- companyName</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1100"/>
+            <a:t>- address1</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1100"/>
+            <a:t>- address</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-CA" sz="1100" baseline="0"/>
@@ -1543,37 +1549,37 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-CA" sz="1100" baseline="0"/>
-            <a:t>- City</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-CA" sz="1100" baseline="0"/>
-            <a:t>- Province</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-CA" sz="1100" baseline="0"/>
-            <a:t>- PostalCode</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-CA" sz="1100" baseline="0"/>
-            <a:t>- PhoneNumber</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-CA" sz="1100" baseline="0"/>
-            <a:t>- ContactPerson</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-CA" sz="1100"/>
-            <a:t>- Contact</a:t>
+            <a:t>- city</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1100" baseline="0"/>
+            <a:t>- province</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1100" baseline="0"/>
+            <a:t>- postalCode</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1100" baseline="0"/>
+            <a:t>- phoneNumber</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1100" baseline="0"/>
+            <a:t>- contactPerson</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1100"/>
+            <a:t>- contact</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-CA" sz="1100" baseline="0"/>
@@ -1584,19 +1590,19 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-CA" sz="1100"/>
-            <a:t>- Active</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-CA" sz="1100"/>
-            <a:t>- DateAdded</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-CA" sz="1100"/>
-            <a:t>- Last</a:t>
+            <a:t>- active</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1100"/>
+            <a:t>- dateAdded</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1100"/>
+            <a:t>- last</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-CA" sz="1100" baseline="0"/>
@@ -1677,49 +1683,49 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-CA" sz="1100"/>
-            <a:t>- ID</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-CA" sz="1100"/>
-            <a:t>- CustomerID</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-CA" sz="1100"/>
-            <a:t>- OrderDate</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-CA" sz="1100"/>
-            <a:t>- Comment</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-CA" sz="1100"/>
-            <a:t>- SalesPersonID</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-CA" sz="1100"/>
-            <a:t>- Active</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-CA" sz="1100"/>
-            <a:t>- DateAdded</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-CA" sz="1100"/>
-            <a:t>- Last</a:t>
+            <a:t>- id</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1100"/>
+            <a:t>- customerId</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1100"/>
+            <a:t>- orderDate</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1100"/>
+            <a:t>- comment</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1100"/>
+            <a:t>- salesPersonId</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1100"/>
+            <a:t>- active</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1100"/>
+            <a:t>- dateAdded</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1100"/>
+            <a:t>- last</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-CA" sz="1100" baseline="0"/>
@@ -1800,43 +1806,43 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-CA" sz="1100"/>
-            <a:t>- ID</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-CA" sz="1100"/>
-            <a:t>- OrderID</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-CA" sz="1100"/>
-            <a:t>- ProductID</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-CA" sz="1100"/>
-            <a:t>- Quantity</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-CA" sz="1100"/>
-            <a:t>- Active</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-CA" sz="1100"/>
-            <a:t>- DateAdded</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-CA" sz="1100"/>
-            <a:t>- Last</a:t>
+            <a:t>- id</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1100"/>
+            <a:t>- orderId</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1100"/>
+            <a:t>- productId</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1100"/>
+            <a:t>- quantity</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1100"/>
+            <a:t>- active</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1100"/>
+            <a:t>- dateAdded</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1100"/>
+            <a:t>- last</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-CA" sz="1100" baseline="0"/>
@@ -1917,19 +1923,19 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-CA" sz="1100"/>
-            <a:t>- ID</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-CA" sz="1100"/>
-            <a:t>- ProductID</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-CA" sz="1100"/>
-            <a:t>- QuantityOn</a:t>
+            <a:t>- id</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1100"/>
+            <a:t>- productId</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1100"/>
+            <a:t>- quantityOn</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-CA" sz="1100" baseline="0"/>
@@ -1939,26 +1945,26 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-CA" sz="1100" baseline="0"/>
-            <a:t>- QuantityTreshold</a:t>
+            <a:t>- quantityTreshold</a:t>
           </a:r>
           <a:endParaRPr lang="en-CA" sz="1100"/>
         </a:p>
         <a:p>
           <a:r>
             <a:rPr lang="en-CA" sz="1100"/>
-            <a:t>- Active</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-CA" sz="1100"/>
-            <a:t>- Date_Added</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-CA" sz="1100"/>
-            <a:t>- Last</a:t>
+            <a:t>- active</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1100"/>
+            <a:t>- date_Added</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1100"/>
+            <a:t>- last</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-CA" sz="1100" baseline="0"/>
@@ -2039,74 +2045,74 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-CA" sz="1100"/>
-            <a:t>- ID</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-CA" sz="1100"/>
-            <a:t>- DeviceID</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-CA" sz="1100"/>
-            <a:t>- CompanyName</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-CA" sz="1100"/>
-            <a:t>- Address1</a:t>
+            <a:t>- id</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1100"/>
+            <a:t>- deviceId</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1100"/>
+            <a:t>- companyName</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1100"/>
+            <a:t>- address1</a:t>
           </a:r>
           <a:endParaRPr lang="en-CA" sz="1100" baseline="0"/>
         </a:p>
         <a:p>
           <a:r>
             <a:rPr lang="en-CA" sz="1100" baseline="0"/>
-            <a:t>- Address2</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-CA" sz="1100"/>
-            <a:t>- City</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-CA" sz="1100"/>
-            <a:t>- Province</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-CA" sz="1100"/>
-            <a:t>- PostalCode</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-CA" sz="1100"/>
-            <a:t>- PhoneNumber</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-CA" sz="1100"/>
-            <a:t>- Active</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-CA" sz="1100"/>
-            <a:t>- DateAdded</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-CA" sz="1100"/>
-            <a:t>- Last</a:t>
+            <a:t>- address2</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1100"/>
+            <a:t>- city</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1100"/>
+            <a:t>- province</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1100"/>
+            <a:t>- postalCode</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1100"/>
+            <a:t>- phoneNumber</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1100"/>
+            <a:t>- active</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1100"/>
+            <a:t>- dateAdded</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1100"/>
+            <a:t>- last</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-CA" sz="1100" baseline="0"/>
@@ -2187,37 +2193,37 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-CA" sz="1100"/>
-            <a:t>- ID</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-CA" sz="1100"/>
-            <a:t>- Name</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-CA" sz="1100"/>
-            <a:t>- Description</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-CA" sz="1100"/>
-            <a:t>- Active</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-CA" sz="1100"/>
-            <a:t>- DateAdded</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-CA" sz="1100"/>
-            <a:t>- Last</a:t>
+            <a:t>- id</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1100"/>
+            <a:t>- name</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1100"/>
+            <a:t>- description</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1100"/>
+            <a:t>- active</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1100"/>
+            <a:t>- dateAdded</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1100"/>
+            <a:t>- last</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-CA" sz="1100" baseline="0"/>
@@ -2298,13 +2304,13 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-CA" sz="1100"/>
-            <a:t>- ID</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-CA" sz="1100"/>
-            <a:t>- Transction</a:t>
+            <a:t>- id</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1100"/>
+            <a:t>- transction</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-CA" sz="1100" baseline="0"/>
@@ -2312,62 +2318,62 @@
           </a:r>
           <a:r>
             <a:rPr lang="en-CA" sz="1100"/>
+            <a:t>Id</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1100"/>
+            <a:t>- order</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1100" baseline="0"/>
             <a:t>ID</a:t>
           </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-CA" sz="1100"/>
-            <a:t>- Order</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-CA" sz="1100" baseline="0"/>
-            <a:t>ID</a:t>
-          </a:r>
           <a:endParaRPr lang="en-CA" sz="1100"/>
         </a:p>
         <a:p>
           <a:r>
             <a:rPr lang="en-CA" sz="1100"/>
-            <a:t>- QuantityOnHand</a:t>
+            <a:t>- quantityOnHand</a:t>
           </a:r>
           <a:endParaRPr lang="en-CA" sz="1100" baseline="0"/>
         </a:p>
         <a:p>
           <a:r>
             <a:rPr lang="en-CA" sz="1100" baseline="0"/>
-            <a:t>- QuantityAdded</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-CA" sz="1100" baseline="0"/>
-            <a:t>- QuantityTaken</a:t>
+            <a:t>- quantityAdded</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1100" baseline="0"/>
+            <a:t>- quantityTaken</a:t>
           </a:r>
           <a:endParaRPr lang="en-CA" sz="1100"/>
         </a:p>
         <a:p>
           <a:r>
             <a:rPr lang="en-CA" sz="1100"/>
-            <a:t>- Active</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-CA" sz="1100"/>
-            <a:t>- UserId</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-CA" sz="1100"/>
-            <a:t>- DateAdded</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-CA" sz="1100"/>
-            <a:t>- Last</a:t>
+            <a:t>- active</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1100"/>
+            <a:t>- userId</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1100"/>
+            <a:t>- dateAdded</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1100"/>
+            <a:t>- last</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-CA" sz="1100" baseline="0"/>
@@ -2448,25 +2454,25 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-CA" sz="1100"/>
-            <a:t>- ID</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-CA" sz="1100"/>
-            <a:t>- Name</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-CA" sz="1100"/>
-            <a:t>- FirstName</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-CA" sz="1100"/>
-            <a:t>- Last</a:t>
+            <a:t>- id</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1100"/>
+            <a:t>- name</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1100"/>
+            <a:t>- firstName</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1100"/>
+            <a:t>- last</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-CA" sz="1100" baseline="0"/>
@@ -2476,32 +2482,32 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-CA" sz="1100" baseline="0"/>
-            <a:t>- LevelID</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-CA" sz="1100" baseline="0"/>
-            <a:t>- Password</a:t>
+            <a:t>- levelId</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1100" baseline="0"/>
+            <a:t>- password</a:t>
           </a:r>
           <a:endParaRPr lang="en-CA" sz="1100"/>
         </a:p>
         <a:p>
           <a:r>
             <a:rPr lang="en-CA" sz="1100"/>
-            <a:t>- Active</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-CA" sz="1100"/>
-            <a:t>- DateAdded</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-CA" sz="1100"/>
-            <a:t>- Last</a:t>
+            <a:t>- active</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1100"/>
+            <a:t>- dateAdded</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1100"/>
+            <a:t>- last</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-CA" sz="1100" baseline="0"/>
@@ -2587,19 +2593,19 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-CA" sz="1100"/>
-            <a:t>- ID</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-CA" sz="1100"/>
-            <a:t>- Name</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-CA" sz="1100"/>
-            <a:t>- Description</a:t>
+            <a:t>- id</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1100"/>
+            <a:t>- name</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1100"/>
+            <a:t>- description</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -2609,26 +2615,26 @@
           </a:r>
           <a:r>
             <a:rPr lang="en-CA" sz="1100" baseline="0"/>
-            <a:t> AuthorityLevel</a:t>
+            <a:t> authorityLevel</a:t>
           </a:r>
           <a:endParaRPr lang="en-CA" sz="1100"/>
         </a:p>
         <a:p>
           <a:r>
             <a:rPr lang="en-CA" sz="1100"/>
-            <a:t>- Active</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-CA" sz="1100"/>
-            <a:t>- DateAdded</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-CA" sz="1100"/>
-            <a:t>- Last</a:t>
+            <a:t>- active</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1100"/>
+            <a:t>- dateAdded</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1100"/>
+            <a:t>- last</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-CA" sz="1100" baseline="0"/>
@@ -2709,37 +2715,37 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-CA" sz="1100"/>
-            <a:t>- ID</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-CA" sz="1100"/>
-            <a:t>- Name</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-CA" sz="1100"/>
-            <a:t>- Description</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-CA" sz="1100"/>
-            <a:t>- Active</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-CA" sz="1100"/>
-            <a:t>- DateAdded</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-CA" sz="1100"/>
-            <a:t>- Last</a:t>
+            <a:t>- id</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1100"/>
+            <a:t>- name</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1100"/>
+            <a:t>- description</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1100"/>
+            <a:t>- active</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1100"/>
+            <a:t>- dateAdded</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1100"/>
+            <a:t>- last</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-CA" sz="1100" baseline="0"/>
@@ -3879,7 +3885,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G10" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="G4" workbookViewId="0">
       <selection activeCell="AG26" sqref="AG26"/>
     </sheetView>
   </sheetViews>

</xml_diff>